<commit_message>
Beging bibliography search screen and data extraction
</commit_message>
<xml_diff>
--- a/input/raw_data/bibliography_search/bib_search_screen_end.xlsx
+++ b/input/raw_data/bibliography_search/bib_search_screen_end.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackgedge/Projects/msc_dissertation/iifo_motivation/input/raw_data/bibliography_search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06E6DE2D-D849-7645-97D3-7D22617FCD91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9E0CD655-8585-8C4C-905E-085305CBE540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="6780" windowWidth="26040" windowHeight="14940" xr2:uid="{2024F0F2-C7A4-0040-8726-2BCD36CB7E46}"/>
+    <workbookView xWindow="20560" yWindow="13080" windowWidth="20560" windowHeight="12220" xr2:uid="{2024F0F2-C7A4-0040-8726-2BCD36CB7E46}"/>
   </bookViews>
   <sheets>
     <sheet name="bib_search_screen_start" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="484">
   <si>
     <t>Study_ID</t>
   </si>
@@ -1361,6 +1361,117 @@
   </si>
   <si>
     <t>Annals of Medicine and Surgery (2012)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical review and case report. Does not report intention. </t>
+  </si>
+  <si>
+    <t>Data_Extracted</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Study_Design</t>
+  </si>
+  <si>
+    <t>Population_Type</t>
+  </si>
+  <si>
+    <t>Study_Setting</t>
+  </si>
+  <si>
+    <t>Study_Location</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>10.1001/jama.1969.03160110135030</t>
+  </si>
+  <si>
+    <t>10.1016/S0002-9610(41)90652-9</t>
+  </si>
+  <si>
+    <t>Case Report</t>
+  </si>
+  <si>
+    <t>New Jersey State Prison Hospital, Trenton</t>
+  </si>
+  <si>
+    <t>Trenton, New Jersey, USA</t>
+  </si>
+  <si>
+    <t>Single prisoner</t>
+  </si>
+  <si>
+    <t>Insertion of pins into thoracic wall</t>
+  </si>
+  <si>
+    <t>No mention of deliberate cases</t>
+  </si>
+  <si>
+    <t>Department of Surgery</t>
+  </si>
+  <si>
+    <t>Berne, Switzerland</t>
+  </si>
+  <si>
+    <t>10.1136/bmj.2.5918.539</t>
+  </si>
+  <si>
+    <t>10.1001/archsurg.1971.01350010016004</t>
+  </si>
+  <si>
+    <t>10.1136/thx.24.2.246</t>
+  </si>
+  <si>
+    <t>10.1001/archsurg.1977.01370050124025</t>
+  </si>
+  <si>
+    <t>New York Medical College-Metropolitan Hospital Center, New York</t>
+  </si>
+  <si>
+    <t>New York, USA</t>
+  </si>
+  <si>
+    <t>Single psychiatric inpatient</t>
+  </si>
+  <si>
+    <t>Retrospective Chart Review</t>
+  </si>
+  <si>
+    <t>General population</t>
+  </si>
+  <si>
+    <t>Queen Mary Hospital</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>10.1002/bjs.1800650103</t>
+  </si>
+  <si>
+    <t>No mention of intention</t>
+  </si>
+  <si>
+    <t>Retrospective Case Series</t>
+  </si>
+  <si>
+    <t>Mixed psychiatric and non-psychiatric</t>
+  </si>
+  <si>
+    <t>Department of Surgery, Charing Cross Hospital,</t>
+  </si>
+  <si>
+    <t>London, UK</t>
+  </si>
+  <si>
+    <t>10.1177/014107688207500207</t>
   </si>
 </sst>
 </file>
@@ -1844,9 +1955,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2222,13 +2334,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A81A345-0683-F840-B0F4-445E0232AC4D}">
-  <dimension ref="A1:N157"/>
+  <dimension ref="A1:T157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2269,10 +2388,28 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>450</v>
+      </c>
+      <c r="O1" t="s">
+        <v>451</v>
+      </c>
+      <c r="P1" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>453</v>
+      </c>
+      <c r="R1" t="s">
+        <v>454</v>
+      </c>
+      <c r="S1" t="s">
+        <v>448</v>
+      </c>
+      <c r="T1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>492</v>
       </c>
@@ -2291,11 +2428,36 @@
       <c r="F2" t="s">
         <v>17</v>
       </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
       <c r="M2" s="1">
         <v>45761.716493055559</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>495</v>
       </c>
@@ -2314,11 +2476,38 @@
       <c r="F3" t="s">
         <v>17</v>
       </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
       <c r="M3" s="1">
         <v>45761.607939814814</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N3" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>496</v>
       </c>
@@ -2337,8 +2526,33 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>45762.43472222222</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="S4" t="s">
+        <v>449</v>
+      </c>
+      <c r="T4" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>497</v>
       </c>
@@ -2357,11 +2571,39 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
       <c r="M5" s="1">
         <v>45761.671574074076</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T5" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>498</v>
       </c>
@@ -2380,8 +2622,41 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>45397.443749999999</v>
+      </c>
+      <c r="N6" t="s">
+        <v>458</v>
+      </c>
+      <c r="O6" t="s">
+        <v>461</v>
+      </c>
+      <c r="P6" t="s">
+        <v>464</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>465</v>
+      </c>
+      <c r="R6" t="s">
+        <v>466</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>499</v>
       </c>
@@ -2400,8 +2675,41 @@
       <c r="F7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
+        <v>45397.447916666664</v>
+      </c>
+      <c r="N7" t="s">
+        <v>458</v>
+      </c>
+      <c r="O7" t="s">
+        <v>472</v>
+      </c>
+      <c r="P7" t="s">
+        <v>470</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>471</v>
+      </c>
+      <c r="R7" t="s">
+        <v>469</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>501</v>
       </c>
@@ -2420,8 +2728,47 @@
       <c r="F8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>9</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>45397.456944444442</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="R8" t="s">
+        <v>477</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>504</v>
       </c>
@@ -2440,8 +2787,41 @@
       <c r="F9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1">
+        <v>45762.482638888891</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="P9" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="R9" t="s">
+        <v>483</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>505</v>
       </c>
@@ -2461,7 +2841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>506</v>
       </c>
@@ -2481,7 +2861,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>507</v>
       </c>
@@ -2503,8 +2883,14 @@
       <c r="M12" s="1">
         <v>45757.375856481478</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>508</v>
       </c>
@@ -2524,7 +2910,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>509</v>
       </c>
@@ -2544,7 +2930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>511</v>
       </c>
@@ -2564,7 +2950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>512</v>
       </c>
@@ -2584,7 +2970,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>514</v>
       </c>
@@ -2604,7 +2990,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>515</v>
       </c>
@@ -2624,7 +3010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>516</v>
       </c>
@@ -2646,8 +3032,14 @@
       <c r="M19" s="1">
         <v>45761.67255787037</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>517</v>
       </c>
@@ -2667,7 +3059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>518</v>
       </c>
@@ -2689,8 +3081,14 @@
       <c r="M21" s="1">
         <v>45761.563564814816</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>520</v>
       </c>
@@ -2710,7 +3108,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>522</v>
       </c>
@@ -2730,7 +3128,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>523</v>
       </c>
@@ -2750,7 +3148,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>524</v>
       </c>
@@ -2772,8 +3170,14 @@
       <c r="M25" s="1">
         <v>45761.540856481479</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>525</v>
       </c>
@@ -2793,7 +3197,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>526</v>
       </c>
@@ -2813,7 +3217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>527</v>
       </c>
@@ -2833,7 +3237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>530</v>
       </c>
@@ -2855,8 +3259,14 @@
       <c r="M29" s="1">
         <v>45761.539814814816</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>532</v>
       </c>
@@ -2876,7 +3286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>533</v>
       </c>
@@ -2896,7 +3306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>534</v>
       </c>
@@ -2916,7 +3326,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>535</v>
       </c>
@@ -2936,7 +3346,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>536</v>
       </c>
@@ -2958,8 +3368,14 @@
       <c r="M34" s="1">
         <v>45761.607071759259</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>537</v>
       </c>
@@ -2979,7 +3395,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>539</v>
       </c>
@@ -3001,8 +3417,14 @@
       <c r="M36" s="1">
         <v>45761.687175925923</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>541</v>
       </c>
@@ -3024,8 +3446,14 @@
       <c r="M37" s="1">
         <v>45761.671203703707</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>542</v>
       </c>
@@ -3045,7 +3473,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>543</v>
       </c>
@@ -3065,7 +3493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>544</v>
       </c>
@@ -3085,7 +3513,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>546</v>
       </c>
@@ -3105,7 +3533,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>547</v>
       </c>
@@ -3125,7 +3553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>548</v>
       </c>
@@ -3145,7 +3573,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>549</v>
       </c>
@@ -3165,7 +3593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>550</v>
       </c>
@@ -3185,7 +3613,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>551</v>
       </c>
@@ -3205,7 +3633,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>552</v>
       </c>
@@ -3225,7 +3653,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>553</v>
       </c>
@@ -3247,8 +3675,14 @@
       <c r="M48" s="1">
         <v>45761.541284722225</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>554</v>
       </c>
@@ -3268,7 +3702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>555</v>
       </c>
@@ -3288,7 +3722,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>556</v>
       </c>
@@ -3308,7 +3742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>557</v>
       </c>
@@ -3328,7 +3762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>558</v>
       </c>
@@ -3348,7 +3782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>559</v>
       </c>
@@ -3368,7 +3802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>561</v>
       </c>
@@ -3388,7 +3822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>562</v>
       </c>
@@ -3408,7 +3842,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>563</v>
       </c>
@@ -3428,7 +3862,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>565</v>
       </c>
@@ -3448,7 +3882,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>566</v>
       </c>
@@ -3468,7 +3902,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>567</v>
       </c>
@@ -3488,7 +3922,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>568</v>
       </c>
@@ -3508,7 +3942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>569</v>
       </c>
@@ -3528,7 +3962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>570</v>
       </c>
@@ -3550,8 +3984,14 @@
       <c r="M63" s="1">
         <v>45761.67496527778</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>572</v>
       </c>
@@ -3571,7 +4011,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>573</v>
       </c>
@@ -3593,8 +4033,14 @@
       <c r="M65" s="1">
         <v>45761.588125000002</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>574</v>
       </c>
@@ -3614,7 +4060,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>575</v>
       </c>
@@ -3634,7 +4080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>576</v>
       </c>
@@ -3656,8 +4102,14 @@
       <c r="M68" s="1">
         <v>45761.61440972222</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>577</v>
       </c>
@@ -3677,7 +4129,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>578</v>
       </c>
@@ -3697,7 +4149,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>579</v>
       </c>
@@ -3717,7 +4169,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>580</v>
       </c>
@@ -3737,7 +4189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>581</v>
       </c>
@@ -3759,8 +4211,14 @@
       <c r="M73" s="1">
         <v>45761.694710648146</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>584</v>
       </c>
@@ -3780,7 +4238,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>585</v>
       </c>
@@ -3800,7 +4258,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>586</v>
       </c>
@@ -3820,7 +4278,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>587</v>
       </c>
@@ -3840,7 +4298,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>588</v>
       </c>
@@ -3860,7 +4318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>589</v>
       </c>
@@ -3880,7 +4338,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>590</v>
       </c>
@@ -3902,8 +4360,14 @@
       <c r="M80" s="1">
         <v>45757.349930555552</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="1"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>591</v>
       </c>
@@ -3923,7 +4387,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>592</v>
       </c>
@@ -3945,8 +4409,14 @@
       <c r="M82" s="1">
         <v>45761.561400462961</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+      <c r="S82" s="1"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>593</v>
       </c>
@@ -3966,7 +4436,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>594</v>
       </c>
@@ -3988,8 +4458,14 @@
       <c r="M84" s="1">
         <v>45761.562210648146</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
+      <c r="S84" s="1"/>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>597</v>
       </c>
@@ -4009,7 +4485,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>598</v>
       </c>
@@ -4029,7 +4505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>600</v>
       </c>
@@ -4049,7 +4525,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>601</v>
       </c>
@@ -4069,7 +4545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>605</v>
       </c>
@@ -4089,7 +4565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>607</v>
       </c>
@@ -4109,7 +4585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>608</v>
       </c>
@@ -4129,7 +4605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>609</v>
       </c>
@@ -4151,8 +4627,14 @@
       <c r="M92" s="1">
         <v>45761.757037037038</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="1"/>
+      <c r="S92" s="1"/>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>611</v>
       </c>
@@ -4172,7 +4654,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>612</v>
       </c>
@@ -4192,7 +4674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>613</v>
       </c>
@@ -4212,7 +4694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>615</v>
       </c>
@@ -4234,8 +4716,14 @@
       <c r="M96" s="1">
         <v>45761.600775462961</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="1"/>
+      <c r="S96" s="1"/>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>616</v>
       </c>
@@ -4255,7 +4743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>617</v>
       </c>
@@ -4277,8 +4765,14 @@
       <c r="M98" s="1">
         <v>45761.611886574072</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1"/>
+      <c r="R98" s="1"/>
+      <c r="S98" s="1"/>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>618</v>
       </c>
@@ -4298,7 +4792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>619</v>
       </c>
@@ -4318,7 +4812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>620</v>
       </c>
@@ -4340,8 +4834,14 @@
       <c r="M101" s="1">
         <v>45761.601111111115</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="1"/>
+      <c r="S101" s="1"/>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>621</v>
       </c>
@@ -4363,8 +4863,14 @@
       <c r="M102" s="1">
         <v>45761.562430555554</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+      <c r="S102" s="1"/>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>622</v>
       </c>
@@ -4384,7 +4890,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>623</v>
       </c>
@@ -4404,7 +4910,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>624</v>
       </c>
@@ -4426,8 +4932,14 @@
       <c r="M105" s="1">
         <v>45761.593888888892</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N105" s="1"/>
+      <c r="O105" s="1"/>
+      <c r="P105" s="1"/>
+      <c r="Q105" s="1"/>
+      <c r="R105" s="1"/>
+      <c r="S105" s="1"/>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>625</v>
       </c>
@@ -4449,8 +4961,14 @@
       <c r="M106" s="1">
         <v>45761.608206018522</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N106" s="1"/>
+      <c r="O106" s="1"/>
+      <c r="P106" s="1"/>
+      <c r="Q106" s="1"/>
+      <c r="R106" s="1"/>
+      <c r="S106" s="1"/>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>627</v>
       </c>
@@ -4470,7 +4988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>628</v>
       </c>
@@ -4492,8 +5010,14 @@
       <c r="M108" s="1">
         <v>45761.552025462966</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N108" s="1"/>
+      <c r="O108" s="1"/>
+      <c r="P108" s="1"/>
+      <c r="Q108" s="1"/>
+      <c r="R108" s="1"/>
+      <c r="S108" s="1"/>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>629</v>
       </c>
@@ -4513,7 +5037,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>630</v>
       </c>
@@ -4533,7 +5057,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>631</v>
       </c>
@@ -4553,7 +5077,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>635</v>
       </c>
@@ -4573,7 +5097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>637</v>
       </c>
@@ -4593,7 +5117,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>638</v>
       </c>
@@ -4613,7 +5137,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>639</v>
       </c>
@@ -4635,8 +5159,14 @@
       <c r="M115" s="1">
         <v>45761.541678240741</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N115" s="1"/>
+      <c r="O115" s="1"/>
+      <c r="P115" s="1"/>
+      <c r="Q115" s="1"/>
+      <c r="R115" s="1"/>
+      <c r="S115" s="1"/>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>640</v>
       </c>
@@ -4658,8 +5188,14 @@
       <c r="M116" s="1">
         <v>45761.562893518516</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N116" s="1"/>
+      <c r="O116" s="1"/>
+      <c r="P116" s="1"/>
+      <c r="Q116" s="1"/>
+      <c r="R116" s="1"/>
+      <c r="S116" s="1"/>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>641</v>
       </c>
@@ -4681,8 +5217,14 @@
       <c r="M117" s="1">
         <v>45761.675127314818</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N117" s="1"/>
+      <c r="O117" s="1"/>
+      <c r="P117" s="1"/>
+      <c r="Q117" s="1"/>
+      <c r="R117" s="1"/>
+      <c r="S117" s="1"/>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>642</v>
       </c>
@@ -4704,8 +5246,14 @@
       <c r="M118" s="1">
         <v>45746.42459490741</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N118" s="1"/>
+      <c r="O118" s="1"/>
+      <c r="P118" s="1"/>
+      <c r="Q118" s="1"/>
+      <c r="R118" s="1"/>
+      <c r="S118" s="1"/>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>643</v>
       </c>
@@ -4725,7 +5273,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>644</v>
       </c>
@@ -4747,8 +5295,14 @@
       <c r="M120" s="1">
         <v>45761.614166666666</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N120" s="1"/>
+      <c r="O120" s="1"/>
+      <c r="P120" s="1"/>
+      <c r="Q120" s="1"/>
+      <c r="R120" s="1"/>
+      <c r="S120" s="1"/>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>645</v>
       </c>
@@ -4768,7 +5322,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>646</v>
       </c>
@@ -4790,8 +5344,14 @@
       <c r="M122" s="1">
         <v>45761.61246527778</v>
       </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N122" s="1"/>
+      <c r="O122" s="1"/>
+      <c r="P122" s="1"/>
+      <c r="Q122" s="1"/>
+      <c r="R122" s="1"/>
+      <c r="S122" s="1"/>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>647</v>
       </c>
@@ -4811,7 +5371,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>648</v>
       </c>
@@ -4833,8 +5393,14 @@
       <c r="M124" s="1">
         <v>45761.58326388889</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N124" s="1"/>
+      <c r="O124" s="1"/>
+      <c r="P124" s="1"/>
+      <c r="Q124" s="1"/>
+      <c r="R124" s="1"/>
+      <c r="S124" s="1"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>649</v>
       </c>
@@ -4856,8 +5422,14 @@
       <c r="M125" s="1">
         <v>45761.574907407405</v>
       </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N125" s="1"/>
+      <c r="O125" s="1"/>
+      <c r="P125" s="1"/>
+      <c r="Q125" s="1"/>
+      <c r="R125" s="1"/>
+      <c r="S125" s="1"/>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>650</v>
       </c>
@@ -4879,8 +5451,14 @@
       <c r="M126" s="1">
         <v>45761.453923611109</v>
       </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N126" s="1"/>
+      <c r="O126" s="1"/>
+      <c r="P126" s="1"/>
+      <c r="Q126" s="1"/>
+      <c r="R126" s="1"/>
+      <c r="S126" s="1"/>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>651</v>
       </c>
@@ -4900,7 +5478,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>652</v>
       </c>
@@ -4922,8 +5500,14 @@
       <c r="M128" s="1">
         <v>45761.581875000003</v>
       </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N128" s="1"/>
+      <c r="O128" s="1"/>
+      <c r="P128" s="1"/>
+      <c r="Q128" s="1"/>
+      <c r="R128" s="1"/>
+      <c r="S128" s="1"/>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>653</v>
       </c>
@@ -4943,7 +5527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>654</v>
       </c>
@@ -4965,8 +5549,14 @@
       <c r="M130" s="1">
         <v>45761.575787037036</v>
       </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N130" s="1"/>
+      <c r="O130" s="1"/>
+      <c r="P130" s="1"/>
+      <c r="Q130" s="1"/>
+      <c r="R130" s="1"/>
+      <c r="S130" s="1"/>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>656</v>
       </c>
@@ -4986,7 +5576,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>657</v>
       </c>
@@ -5008,8 +5598,14 @@
       <c r="M132" s="1">
         <v>45761.584166666667</v>
       </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N132" s="1"/>
+      <c r="O132" s="1"/>
+      <c r="P132" s="1"/>
+      <c r="Q132" s="1"/>
+      <c r="R132" s="1"/>
+      <c r="S132" s="1"/>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>658</v>
       </c>
@@ -5029,7 +5625,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>660</v>
       </c>
@@ -5049,7 +5645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>662</v>
       </c>
@@ -5069,7 +5665,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>663</v>
       </c>
@@ -5089,7 +5685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>664</v>
       </c>
@@ -5109,7 +5705,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>665</v>
       </c>
@@ -5129,7 +5725,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>667</v>
       </c>
@@ -5148,8 +5744,14 @@
       <c r="M139" s="1">
         <v>45761.529270833336</v>
       </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N139" s="1"/>
+      <c r="O139" s="1"/>
+      <c r="P139" s="1"/>
+      <c r="Q139" s="1"/>
+      <c r="R139" s="1"/>
+      <c r="S139" s="1"/>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>669</v>
       </c>
@@ -5171,8 +5773,14 @@
       <c r="M140" s="1">
         <v>45761.572060185186</v>
       </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N140" s="1"/>
+      <c r="O140" s="1"/>
+      <c r="P140" s="1"/>
+      <c r="Q140" s="1"/>
+      <c r="R140" s="1"/>
+      <c r="S140" s="1"/>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>670</v>
       </c>
@@ -5192,7 +5800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>672</v>
       </c>
@@ -5214,8 +5822,14 @@
       <c r="M142" s="1">
         <v>45761.581365740742</v>
       </c>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N142" s="1"/>
+      <c r="O142" s="1"/>
+      <c r="P142" s="1"/>
+      <c r="Q142" s="1"/>
+      <c r="R142" s="1"/>
+      <c r="S142" s="1"/>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>673</v>
       </c>
@@ -5235,7 +5849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>674</v>
       </c>
@@ -5255,7 +5869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>675</v>
       </c>
@@ -5277,8 +5891,14 @@
       <c r="M145" s="1">
         <v>45746.429988425924</v>
       </c>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N145" s="1"/>
+      <c r="O145" s="1"/>
+      <c r="P145" s="1"/>
+      <c r="Q145" s="1"/>
+      <c r="R145" s="1"/>
+      <c r="S145" s="1"/>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>676</v>
       </c>
@@ -5300,8 +5920,14 @@
       <c r="M146" s="1">
         <v>45761.581712962965</v>
       </c>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N146" s="1"/>
+      <c r="O146" s="1"/>
+      <c r="P146" s="1"/>
+      <c r="Q146" s="1"/>
+      <c r="R146" s="1"/>
+      <c r="S146" s="1"/>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>677</v>
       </c>
@@ -5323,8 +5949,14 @@
       <c r="M147" s="1">
         <v>45761.53769675926</v>
       </c>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N147" s="1"/>
+      <c r="O147" s="1"/>
+      <c r="P147" s="1"/>
+      <c r="Q147" s="1"/>
+      <c r="R147" s="1"/>
+      <c r="S147" s="1"/>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>678</v>
       </c>
@@ -5346,8 +5978,14 @@
       <c r="M148" s="1">
         <v>45746.438900462963</v>
       </c>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N148" s="1"/>
+      <c r="O148" s="1"/>
+      <c r="P148" s="1"/>
+      <c r="Q148" s="1"/>
+      <c r="R148" s="1"/>
+      <c r="S148" s="1"/>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>679</v>
       </c>
@@ -5367,7 +6005,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>680</v>
       </c>
@@ -5387,7 +6025,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>681</v>
       </c>
@@ -5409,8 +6047,14 @@
       <c r="M151" s="1">
         <v>45761.526678240742</v>
       </c>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N151" s="1"/>
+      <c r="O151" s="1"/>
+      <c r="P151" s="1"/>
+      <c r="Q151" s="1"/>
+      <c r="R151" s="1"/>
+      <c r="S151" s="1"/>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>682</v>
       </c>
@@ -5430,7 +6074,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>683</v>
       </c>
@@ -5452,8 +6096,14 @@
       <c r="M153" s="1">
         <v>45761.590138888889</v>
       </c>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N153" s="1"/>
+      <c r="O153" s="1"/>
+      <c r="P153" s="1"/>
+      <c r="Q153" s="1"/>
+      <c r="R153" s="1"/>
+      <c r="S153" s="1"/>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>684</v>
       </c>
@@ -5475,8 +6125,14 @@
       <c r="M154" s="1">
         <v>45761.527395833335</v>
       </c>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N154" s="1"/>
+      <c r="O154" s="1"/>
+      <c r="P154" s="1"/>
+      <c r="Q154" s="1"/>
+      <c r="R154" s="1"/>
+      <c r="S154" s="1"/>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>686</v>
       </c>
@@ -5498,8 +6154,14 @@
       <c r="M155" s="1">
         <v>45746.432546296295</v>
       </c>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N155" s="1"/>
+      <c r="O155" s="1"/>
+      <c r="P155" s="1"/>
+      <c r="Q155" s="1"/>
+      <c r="R155" s="1"/>
+      <c r="S155" s="1"/>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>687</v>
       </c>
@@ -5521,8 +6183,14 @@
       <c r="M156" s="1">
         <v>45746.431377314817</v>
       </c>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N156" s="1"/>
+      <c r="O156" s="1"/>
+      <c r="P156" s="1"/>
+      <c r="Q156" s="1"/>
+      <c r="R156" s="1"/>
+      <c r="S156" s="1"/>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>688</v>
       </c>

</xml_diff>

<commit_message>
Continued bibliography search data extraction
</commit_message>
<xml_diff>
--- a/input/raw_data/bibliography_search/bib_search_screen_end.xlsx
+++ b/input/raw_data/bibliography_search/bib_search_screen_end.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackgedge/Projects/msc_dissertation/iifo_motivation/input/raw_data/bibliography_search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9E0CD655-8585-8C4C-905E-085305CBE540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2F1205EA-3FA6-D54F-9029-442B42EBFEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20560" yWindow="13080" windowWidth="20560" windowHeight="12220" xr2:uid="{2024F0F2-C7A4-0040-8726-2BCD36CB7E46}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="544">
   <si>
     <t>Study_ID</t>
   </si>
@@ -1472,6 +1472,186 @@
   </si>
   <si>
     <t>10.1177/014107688207500207</t>
+  </si>
+  <si>
+    <t>Single psychiatric patient</t>
+  </si>
+  <si>
+    <t>Tulane University School of Medicine</t>
+  </si>
+  <si>
+    <t>New Orleans, Lousiana, USA</t>
+  </si>
+  <si>
+    <t>10.1016/s0016-5107(83)72564-2</t>
+  </si>
+  <si>
+    <t>Non-intentional - "swallowing a toothbrush during one of his seizure episodes"</t>
+  </si>
+  <si>
+    <t>Single psychiatric prisoner</t>
+  </si>
+  <si>
+    <t>Miami School of Medicine</t>
+  </si>
+  <si>
+    <t>Miami, Florida, USA</t>
+  </si>
+  <si>
+    <t>10.1097/00005053-198305000-00012</t>
+  </si>
+  <si>
+    <t>Does not report outcomes for individual ingestions.</t>
+  </si>
+  <si>
+    <t>University of Texas</t>
+  </si>
+  <si>
+    <t>Galveston, Texas, USA</t>
+  </si>
+  <si>
+    <t>10.1097/00007611-198309000-00015</t>
+  </si>
+  <si>
+    <t>Psychiatric patients</t>
+  </si>
+  <si>
+    <t>Mixed intentional, non-intentional and food bolus. No information on rates of intentional ingestion so unable to differentiate empirical data. Exclude.</t>
+  </si>
+  <si>
+    <t>Tampa General Hospital and the James A. Haley Veterans Hospital</t>
+  </si>
+  <si>
+    <t>All patients with a foreign body of the upper gastrointestinal tract endoscopically</t>
+  </si>
+  <si>
+    <t>Tampa, Florida, USA</t>
+  </si>
+  <si>
+    <t>10.1016/s0016-5107(83)72586-1</t>
+  </si>
+  <si>
+    <t>University of California, Davis, Medical Center</t>
+  </si>
+  <si>
+    <t>Davis, California, USA</t>
+  </si>
+  <si>
+    <t>10.1016/s0196-0644(84)80380-7</t>
+  </si>
+  <si>
+    <t>Mixed population, adult and child with inteional and non-intentional ingestion</t>
+  </si>
+  <si>
+    <t>10.1016/s0016-5107(86)71926-3</t>
+  </si>
+  <si>
+    <t>10.1097/00000658-198402000-00010</t>
+  </si>
+  <si>
+    <t>Not explicitly intentional - "ahistory of ingestion of aquarter 20 years previously was elicited."</t>
+  </si>
+  <si>
+    <t>Case Series</t>
+  </si>
+  <si>
+    <t>All accidental</t>
+  </si>
+  <si>
+    <t>10.1001/archsurg.1988.01400270122020</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Accidental</t>
+  </si>
+  <si>
+    <t>10.1097/00006565-198812000-00004</t>
+  </si>
+  <si>
+    <t>Bib_Search_Complete</t>
+  </si>
+  <si>
+    <t>10.1111/j.1440-1673.1988.tb02755.x</t>
+  </si>
+  <si>
+    <t>10.1016/0016-5085(88)90632-4</t>
+  </si>
+  <si>
+    <t>Review, no empirical evidence</t>
+  </si>
+  <si>
+    <t>Not explicitly intentional</t>
+  </si>
+  <si>
+    <t>10.1097/00000433-199012000-00014</t>
+  </si>
+  <si>
+    <t>Co-existing mechanism of death - "death was attributed to cardiorespiratory arrest in delayed shock accompanying peritonitis and mechanical obstruction of the airways"</t>
+  </si>
+  <si>
+    <t>10.1148/radiology.174.1.2294547</t>
+  </si>
+  <si>
+    <t>Intention not reported. Likely mixed cohort. Exclude.</t>
+  </si>
+  <si>
+    <t>10.1007/BF01665320</t>
+  </si>
+  <si>
+    <t>The Gregorio Marafirn Memorial Hospital</t>
+  </si>
+  <si>
+    <t>Madrid, Spain</t>
+  </si>
+  <si>
+    <t>Mixed population</t>
+  </si>
+  <si>
+    <t>all patients (N= 19) admitted to a medical prison ward for men in a New York City public general hospital for delib erately swallowing objects between September 1, 1985, and October 15,</t>
+  </si>
+  <si>
+    <t>New York City Public General Hospital</t>
+  </si>
+  <si>
+    <t>10.1176/ps.42.5.533</t>
+  </si>
+  <si>
+    <t>10.1016/S0025-7125(16)30212-7</t>
+  </si>
+  <si>
+    <t>10.1097/00063110-199506000-00005</t>
+  </si>
+  <si>
+    <t>COPROPHAGIA  = eatings ones own faeces. Exclude.</t>
+  </si>
+  <si>
+    <t>10.1016/0005-7916(94)00065-t</t>
+  </si>
+  <si>
+    <t>10.1007/s002689900152</t>
+  </si>
+  <si>
+    <t>10.1155/1997/815876</t>
+  </si>
+  <si>
+    <t>Patients with occult liver abscess</t>
+  </si>
+  <si>
+    <t>Royal Alexandra Hospital</t>
+  </si>
+  <si>
+    <t>Edmonton, Alberta, Canada</t>
+  </si>
+  <si>
+    <t>One intentional, one unitentional</t>
+  </si>
+  <si>
+    <t>Accidental - "A 20-year-old Asian female presented to the emergency room complaining of having swallowed her toothbrush. She stated that she had been attempting to scratch her pharynx with the handle of her toothbrush when a spontaneous gag reflex caused her to swallow the toothbrush"</t>
+  </si>
+  <si>
+    <t>10.1007/s004649900393</t>
   </si>
 </sst>
 </file>
@@ -2334,20 +2514,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A81A345-0683-F840-B0F4-445E0232AC4D}">
-  <dimension ref="A1:T157"/>
+  <dimension ref="A1:U157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="15.33203125" customWidth="1"/>
+    <col min="14" max="20" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2406,10 +2586,13 @@
         <v>448</v>
       </c>
       <c r="T1" t="s">
+        <v>516</v>
+      </c>
+      <c r="U1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>492</v>
       </c>
@@ -2453,11 +2636,14 @@
       <c r="S2" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>495</v>
       </c>
@@ -2506,8 +2692,11 @@
       <c r="S3" s="1" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T3" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>496</v>
       </c>
@@ -2548,11 +2737,14 @@
       <c r="S4" t="s">
         <v>449</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U4" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>497</v>
       </c>
@@ -2599,11 +2791,14 @@
       <c r="S5" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U5" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>498</v>
       </c>
@@ -2655,8 +2850,11 @@
       <c r="S6" s="1" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T6" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>499</v>
       </c>
@@ -2708,8 +2906,11 @@
       <c r="S7" s="1" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T7" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>501</v>
       </c>
@@ -2765,10 +2966,13 @@
         <v>449</v>
       </c>
       <c r="T8" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U8" s="1" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>504</v>
       </c>
@@ -2820,8 +3024,11 @@
       <c r="S9" s="1" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T9" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>505</v>
       </c>
@@ -2840,8 +3047,50 @@
       <c r="F10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>45762.489583333336</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="P10" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="R10" t="s">
+        <v>487</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U10" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>506</v>
       </c>
@@ -2860,8 +3109,50 @@
       <c r="F11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2">
+        <v>45762.495138888888</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="P11" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>491</v>
+      </c>
+      <c r="R11" t="s">
+        <v>492</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U11" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>507</v>
       </c>
@@ -2880,17 +3171,41 @@
       <c r="F12" t="s">
         <v>17</v>
       </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
       <c r="M12" s="1">
         <v>45757.375856481478</v>
       </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N12" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>508</v>
       </c>
@@ -2909,8 +3224,44 @@
       <c r="F13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>45762.506249999999</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="O13" t="s">
+        <v>500</v>
+      </c>
+      <c r="P13" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="R13" t="s">
+        <v>502</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U13" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>509</v>
       </c>
@@ -2929,8 +3280,44 @@
       <c r="F14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1">
+        <v>45762.508333333331</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="O14" t="s">
+        <v>506</v>
+      </c>
+      <c r="P14" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="R14" t="s">
+        <v>505</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>511</v>
       </c>
@@ -2949,8 +3336,32 @@
       <c r="F15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>9</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>45762.557638888888</v>
+      </c>
+      <c r="R15" t="s">
+        <v>508</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>512</v>
       </c>
@@ -2969,8 +3380,38 @@
       <c r="F16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>9</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>45762.581944444442</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="R16" t="s">
+        <v>507</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U16" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>514</v>
       </c>
@@ -2989,8 +3430,38 @@
       <c r="F17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>45762.586111111108</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="R17" t="s">
+        <v>512</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U17" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>515</v>
       </c>
@@ -3009,8 +3480,41 @@
       <c r="F18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>45762.587500000001</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="R18" t="s">
+        <v>515</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U18" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>516</v>
       </c>
@@ -3029,17 +3533,41 @@
       <c r="F19" t="s">
         <v>17</v>
       </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>9</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <v>0</v>
+      </c>
       <c r="M19" s="1">
-        <v>45761.67255787037</v>
-      </c>
-      <c r="N19" s="1"/>
+        <v>45762.590277777781</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>458</v>
+      </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R19" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>517</v>
       </c>
@@ -3058,8 +3586,38 @@
       <c r="F20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>45762.591666666667</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="R20" t="s">
+        <v>518</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U20" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>518</v>
       </c>
@@ -3078,17 +3636,41 @@
       <c r="F21" t="s">
         <v>17</v>
       </c>
-      <c r="M21" s="1">
-        <v>45761.563564814816</v>
-      </c>
-      <c r="N21" s="1"/>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>11</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2">
+        <v>45762.592361111114</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>458</v>
+      </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R21" t="s">
+        <v>521</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U21" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>520</v>
       </c>
@@ -3107,8 +3689,38 @@
       <c r="F22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>9</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>45762.599305555559</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="R22" t="s">
+        <v>523</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U22" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>522</v>
       </c>
@@ -3127,8 +3739,41 @@
       <c r="F23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1">
+        <v>45762.602777777778</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="O23" t="s">
+        <v>528</v>
+      </c>
+      <c r="P23" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>527</v>
+      </c>
+      <c r="R23" t="s">
+        <v>525</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>523</v>
       </c>
@@ -3147,8 +3792,41 @@
       <c r="F24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" s="1">
+        <v>45762.635416666664</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="O24" t="s">
+        <v>529</v>
+      </c>
+      <c r="P24" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>471</v>
+      </c>
+      <c r="R24" t="s">
+        <v>531</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>524</v>
       </c>
@@ -3167,17 +3845,35 @@
       <c r="F25" t="s">
         <v>17</v>
       </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
       <c r="M25" s="1">
         <v>45761.540856481479</v>
       </c>
-      <c r="N25" s="1"/>
+      <c r="N25" s="1" t="s">
+        <v>513</v>
+      </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R25" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>525</v>
       </c>
@@ -3196,8 +3892,41 @@
       <c r="F26" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>9</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="b">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>45397.660416666666</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="R26" t="s">
+        <v>533</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U26" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>526</v>
       </c>
@@ -3216,8 +3945,32 @@
       <c r="F27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>9</v>
+      </c>
+      <c r="M27" s="1">
+        <v>45762.663194444445</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="R27" t="s">
+        <v>533</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U27" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>527</v>
       </c>
@@ -3236,8 +3989,35 @@
       <c r="F28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>7</v>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1">
+        <v>45762.665277777778</v>
+      </c>
+      <c r="R28" t="s">
+        <v>535</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U28" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>530</v>
       </c>
@@ -3256,17 +4036,38 @@
       <c r="F29" t="s">
         <v>17</v>
       </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>9</v>
+      </c>
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
       <c r="M29" s="1">
         <v>45761.539814814816</v>
       </c>
-      <c r="N29" s="1"/>
+      <c r="N29" s="1" t="s">
+        <v>473</v>
+      </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R29" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>532</v>
       </c>
@@ -3285,8 +4086,44 @@
       <c r="F30" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M30" s="1">
+        <v>45762.675694444442</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="O30" t="s">
+        <v>538</v>
+      </c>
+      <c r="P30" t="s">
+        <v>539</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>540</v>
+      </c>
+      <c r="R30" t="s">
+        <v>537</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U30" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>533</v>
       </c>
@@ -3305,8 +4142,29 @@
       <c r="F31" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="M31" s="1">
+        <v>45762.677777777775</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="R31" t="s">
+        <v>543</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="U31" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>534</v>
       </c>
@@ -3325,8 +4183,11 @@
       <c r="F32" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T32" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>535</v>
       </c>
@@ -3345,8 +4206,11 @@
       <c r="F33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T33" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>536</v>
       </c>
@@ -3374,8 +4238,11 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T34" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>537</v>
       </c>
@@ -3394,8 +4261,11 @@
       <c r="F35" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T35" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>539</v>
       </c>
@@ -3423,8 +4293,11 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T36" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>541</v>
       </c>
@@ -3452,8 +4325,11 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T37" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>542</v>
       </c>
@@ -3472,8 +4348,11 @@
       <c r="F38" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T38" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>543</v>
       </c>
@@ -3492,8 +4371,11 @@
       <c r="F39" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T39" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>544</v>
       </c>
@@ -3512,8 +4394,11 @@
       <c r="F40" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T40" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>546</v>
       </c>
@@ -3532,8 +4417,11 @@
       <c r="F41" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T41" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>547</v>
       </c>
@@ -3552,8 +4440,11 @@
       <c r="F42" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T42" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>548</v>
       </c>
@@ -3572,8 +4463,11 @@
       <c r="F43" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T43" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>549</v>
       </c>
@@ -3592,8 +4486,11 @@
       <c r="F44" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T44" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>550</v>
       </c>
@@ -3612,8 +4509,11 @@
       <c r="F45" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T45" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>551</v>
       </c>
@@ -3632,8 +4532,11 @@
       <c r="F46" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T46" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>552</v>
       </c>
@@ -3652,8 +4555,11 @@
       <c r="F47" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T47" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>553</v>
       </c>
@@ -3681,8 +4587,11 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T48" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>554</v>
       </c>
@@ -3701,8 +4610,11 @@
       <c r="F49" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T49" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>555</v>
       </c>
@@ -3721,8 +4633,11 @@
       <c r="F50" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T50" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>556</v>
       </c>
@@ -3741,8 +4656,11 @@
       <c r="F51" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T51" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>557</v>
       </c>
@@ -3761,8 +4679,11 @@
       <c r="F52" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T52" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>558</v>
       </c>
@@ -3781,8 +4702,11 @@
       <c r="F53" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T53" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>559</v>
       </c>
@@ -3801,8 +4725,11 @@
       <c r="F54" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T54" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>561</v>
       </c>
@@ -3821,8 +4748,11 @@
       <c r="F55" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T55" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>562</v>
       </c>
@@ -3841,8 +4771,11 @@
       <c r="F56" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T56" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>563</v>
       </c>
@@ -3861,8 +4794,11 @@
       <c r="F57" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T57" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>565</v>
       </c>
@@ -3881,8 +4817,11 @@
       <c r="F58" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T58" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>566</v>
       </c>
@@ -3901,8 +4840,11 @@
       <c r="F59" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T59" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>567</v>
       </c>
@@ -3921,8 +4863,11 @@
       <c r="F60" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T60" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>568</v>
       </c>
@@ -3941,8 +4886,11 @@
       <c r="F61" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T61" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>569</v>
       </c>
@@ -3961,8 +4909,11 @@
       <c r="F62" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T62" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>570</v>
       </c>
@@ -3990,8 +4941,11 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T63" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>572</v>
       </c>
@@ -4010,8 +4964,11 @@
       <c r="F64" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T64" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>573</v>
       </c>
@@ -4039,8 +4996,11 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T65" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>574</v>
       </c>
@@ -4059,8 +5019,11 @@
       <c r="F66" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T66" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>575</v>
       </c>
@@ -4079,8 +5042,11 @@
       <c r="F67" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T67" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>576</v>
       </c>
@@ -4108,8 +5074,11 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T68" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>577</v>
       </c>
@@ -4128,8 +5097,11 @@
       <c r="F69" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T69" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>578</v>
       </c>
@@ -4148,8 +5120,11 @@
       <c r="F70" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T70" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>579</v>
       </c>
@@ -4168,8 +5143,11 @@
       <c r="F71" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T71" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>580</v>
       </c>
@@ -4188,8 +5166,11 @@
       <c r="F72" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T72" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>581</v>
       </c>
@@ -4217,8 +5198,11 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
       <c r="S73" s="1"/>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T73" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>584</v>
       </c>
@@ -4237,8 +5221,11 @@
       <c r="F74" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T74" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>585</v>
       </c>
@@ -4257,8 +5244,11 @@
       <c r="F75" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T75" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>586</v>
       </c>
@@ -4277,8 +5267,11 @@
       <c r="F76" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T76" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>587</v>
       </c>
@@ -4297,8 +5290,11 @@
       <c r="F77" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T77" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>588</v>
       </c>
@@ -4317,8 +5313,11 @@
       <c r="F78" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T78" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>589</v>
       </c>
@@ -4337,8 +5336,11 @@
       <c r="F79" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T79" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>590</v>
       </c>
@@ -4366,8 +5368,11 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T80" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>591</v>
       </c>
@@ -4386,8 +5391,11 @@
       <c r="F81" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T81" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>592</v>
       </c>
@@ -4415,8 +5423,11 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
       <c r="S82" s="1"/>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T82" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>593</v>
       </c>
@@ -4435,8 +5446,11 @@
       <c r="F83" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T83" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>594</v>
       </c>
@@ -4464,8 +5478,11 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T84" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>597</v>
       </c>
@@ -4484,8 +5501,11 @@
       <c r="F85" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T85" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>598</v>
       </c>
@@ -4504,8 +5524,11 @@
       <c r="F86" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T86" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>600</v>
       </c>
@@ -4524,8 +5547,11 @@
       <c r="F87" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T87" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>601</v>
       </c>
@@ -4544,8 +5570,11 @@
       <c r="F88" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T88" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>605</v>
       </c>
@@ -4564,8 +5593,11 @@
       <c r="F89" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T89" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>607</v>
       </c>
@@ -4584,8 +5616,11 @@
       <c r="F90" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T90" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>608</v>
       </c>
@@ -4604,8 +5639,11 @@
       <c r="F91" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T91" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>609</v>
       </c>
@@ -4633,8 +5671,11 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
       <c r="S92" s="1"/>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T92" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>611</v>
       </c>
@@ -4653,8 +5694,11 @@
       <c r="F93" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T93" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>612</v>
       </c>
@@ -4673,8 +5717,11 @@
       <c r="F94" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T94" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>613</v>
       </c>
@@ -4693,8 +5740,11 @@
       <c r="F95" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T95" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>615</v>
       </c>
@@ -4722,8 +5772,11 @@
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
       <c r="S96" s="1"/>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T96" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>616</v>
       </c>
@@ -4742,8 +5795,11 @@
       <c r="F97" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T97" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>617</v>
       </c>
@@ -4771,8 +5827,11 @@
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
       <c r="S98" s="1"/>
-    </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T98" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>618</v>
       </c>
@@ -4791,8 +5850,11 @@
       <c r="F99" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T99" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>619</v>
       </c>
@@ -4811,8 +5873,11 @@
       <c r="F100" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T100" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>620</v>
       </c>
@@ -4840,8 +5905,11 @@
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
       <c r="S101" s="1"/>
-    </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T101" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>621</v>
       </c>
@@ -4869,8 +5937,11 @@
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
       <c r="S102" s="1"/>
-    </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T102" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>622</v>
       </c>
@@ -4889,8 +5960,11 @@
       <c r="F103" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T103" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>623</v>
       </c>
@@ -4909,8 +5983,11 @@
       <c r="F104" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T104" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>624</v>
       </c>
@@ -4938,8 +6015,11 @@
       <c r="Q105" s="1"/>
       <c r="R105" s="1"/>
       <c r="S105" s="1"/>
-    </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T105" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>625</v>
       </c>
@@ -4967,8 +6047,11 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
       <c r="S106" s="1"/>
-    </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T106" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>627</v>
       </c>
@@ -4987,8 +6070,11 @@
       <c r="F107" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T107" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>628</v>
       </c>
@@ -5016,8 +6102,11 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
       <c r="S108" s="1"/>
-    </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T108" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>629</v>
       </c>
@@ -5036,8 +6125,11 @@
       <c r="F109" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T109" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>630</v>
       </c>
@@ -5056,8 +6148,11 @@
       <c r="F110" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T110" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>631</v>
       </c>
@@ -5076,8 +6171,11 @@
       <c r="F111" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T111" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>635</v>
       </c>
@@ -5096,8 +6194,11 @@
       <c r="F112" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T112" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>637</v>
       </c>
@@ -5116,8 +6217,11 @@
       <c r="F113" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T113" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>638</v>
       </c>
@@ -5136,8 +6240,11 @@
       <c r="F114" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T114" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>639</v>
       </c>
@@ -5165,8 +6272,11 @@
       <c r="Q115" s="1"/>
       <c r="R115" s="1"/>
       <c r="S115" s="1"/>
-    </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T115" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>640</v>
       </c>
@@ -5194,8 +6304,11 @@
       <c r="Q116" s="1"/>
       <c r="R116" s="1"/>
       <c r="S116" s="1"/>
-    </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T116" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>641</v>
       </c>
@@ -5223,8 +6336,11 @@
       <c r="Q117" s="1"/>
       <c r="R117" s="1"/>
       <c r="S117" s="1"/>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T117" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>642</v>
       </c>
@@ -5252,8 +6368,11 @@
       <c r="Q118" s="1"/>
       <c r="R118" s="1"/>
       <c r="S118" s="1"/>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T118" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>643</v>
       </c>
@@ -5272,8 +6391,11 @@
       <c r="F119" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T119" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>644</v>
       </c>
@@ -5301,8 +6423,11 @@
       <c r="Q120" s="1"/>
       <c r="R120" s="1"/>
       <c r="S120" s="1"/>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T120" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>645</v>
       </c>
@@ -5321,8 +6446,11 @@
       <c r="F121" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T121" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>646</v>
       </c>
@@ -5350,8 +6478,11 @@
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
       <c r="S122" s="1"/>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T122" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>647</v>
       </c>
@@ -5370,8 +6501,11 @@
       <c r="F123" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T123" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>648</v>
       </c>
@@ -5399,8 +6533,11 @@
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
       <c r="S124" s="1"/>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T124" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>649</v>
       </c>
@@ -5428,8 +6565,11 @@
       <c r="Q125" s="1"/>
       <c r="R125" s="1"/>
       <c r="S125" s="1"/>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T125" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>650</v>
       </c>
@@ -5457,8 +6597,11 @@
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
       <c r="S126" s="1"/>
-    </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T126" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>651</v>
       </c>
@@ -5477,8 +6620,11 @@
       <c r="F127" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T127" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>652</v>
       </c>
@@ -5506,8 +6652,11 @@
       <c r="Q128" s="1"/>
       <c r="R128" s="1"/>
       <c r="S128" s="1"/>
-    </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T128" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>653</v>
       </c>
@@ -5526,8 +6675,11 @@
       <c r="F129" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T129" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>654</v>
       </c>
@@ -5555,8 +6707,11 @@
       <c r="Q130" s="1"/>
       <c r="R130" s="1"/>
       <c r="S130" s="1"/>
-    </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T130" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>656</v>
       </c>
@@ -5575,8 +6730,11 @@
       <c r="F131" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T131" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>657</v>
       </c>
@@ -5604,8 +6762,11 @@
       <c r="Q132" s="1"/>
       <c r="R132" s="1"/>
       <c r="S132" s="1"/>
-    </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T132" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>658</v>
       </c>
@@ -5624,8 +6785,11 @@
       <c r="F133" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T133" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>660</v>
       </c>
@@ -5644,8 +6808,11 @@
       <c r="F134" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T134" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>662</v>
       </c>
@@ -5664,8 +6831,11 @@
       <c r="F135" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T135" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>663</v>
       </c>
@@ -5684,8 +6854,11 @@
       <c r="F136" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T136" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>664</v>
       </c>
@@ -5704,8 +6877,11 @@
       <c r="F137" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T137" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>665</v>
       </c>
@@ -5724,8 +6900,11 @@
       <c r="F138" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T138" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>667</v>
       </c>
@@ -5750,8 +6929,11 @@
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
       <c r="S139" s="1"/>
-    </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T139" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>669</v>
       </c>
@@ -5779,8 +6961,11 @@
       <c r="Q140" s="1"/>
       <c r="R140" s="1"/>
       <c r="S140" s="1"/>
-    </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T140" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>670</v>
       </c>
@@ -5799,8 +6984,11 @@
       <c r="F141" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T141" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>672</v>
       </c>
@@ -5828,8 +7016,11 @@
       <c r="Q142" s="1"/>
       <c r="R142" s="1"/>
       <c r="S142" s="1"/>
-    </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T142" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>673</v>
       </c>
@@ -5848,8 +7039,11 @@
       <c r="F143" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T143" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>674</v>
       </c>
@@ -5868,8 +7062,11 @@
       <c r="F144" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T144" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>675</v>
       </c>
@@ -5897,8 +7094,11 @@
       <c r="Q145" s="1"/>
       <c r="R145" s="1"/>
       <c r="S145" s="1"/>
-    </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T145" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>676</v>
       </c>
@@ -5926,8 +7126,11 @@
       <c r="Q146" s="1"/>
       <c r="R146" s="1"/>
       <c r="S146" s="1"/>
-    </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T146" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>677</v>
       </c>
@@ -5955,8 +7158,11 @@
       <c r="Q147" s="1"/>
       <c r="R147" s="1"/>
       <c r="S147" s="1"/>
-    </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T147" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="148" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>678</v>
       </c>
@@ -5984,8 +7190,11 @@
       <c r="Q148" s="1"/>
       <c r="R148" s="1"/>
       <c r="S148" s="1"/>
-    </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T148" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>679</v>
       </c>
@@ -6004,8 +7213,11 @@
       <c r="F149" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T149" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>680</v>
       </c>
@@ -6024,8 +7236,11 @@
       <c r="F150" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T150" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>681</v>
       </c>
@@ -6053,8 +7268,11 @@
       <c r="Q151" s="1"/>
       <c r="R151" s="1"/>
       <c r="S151" s="1"/>
-    </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T151" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="152" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>682</v>
       </c>
@@ -6073,8 +7291,11 @@
       <c r="F152" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T152" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="153" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>683</v>
       </c>
@@ -6102,8 +7323,11 @@
       <c r="Q153" s="1"/>
       <c r="R153" s="1"/>
       <c r="S153" s="1"/>
-    </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T153" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="154" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>684</v>
       </c>
@@ -6131,8 +7355,11 @@
       <c r="Q154" s="1"/>
       <c r="R154" s="1"/>
       <c r="S154" s="1"/>
-    </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T154" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="155" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>686</v>
       </c>
@@ -6160,8 +7387,11 @@
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
       <c r="S155" s="1"/>
-    </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T155" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="156" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>687</v>
       </c>
@@ -6189,8 +7419,11 @@
       <c r="Q156" s="1"/>
       <c r="R156" s="1"/>
       <c r="S156" s="1"/>
-    </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T156" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="157" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>688</v>
       </c>
@@ -6208,6 +7441,9 @@
       </c>
       <c r="F157" t="s">
         <v>17</v>
+      </c>
+      <c r="T157" s="1" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>